<commit_message>
Updated with Example to support Kafka and Data base via Low code automation
</commit_message>
<xml_diff>
--- a/samples/idaithalam-db-kafka-apitesting/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
+++ b/samples/idaithalam-db-kafka-apitesting/src/test/resources/virtualan_collection_kafka_db_testcase_0.xlsx
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t xml:space="preserve">pet </t>
+  </si>
+  <si>
+    <t>RequestContents</t>
+  </si>
+  <si>
+    <t>create table employees (emp_no int, birth_date date,first_name VARCHAR(50),last_name VARCHAR(50), gender VARCHAR(50),hire_date date)</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>insert into employees (emp_no,birth_date,first_name,last_name, gender,hire_date) values  (2,'1978-01-08','ELan', 'Thangamani', 'Male', '2007-10-10')</t>
+  </si>
+  <si>
+    <t>RequestContent</t>
   </si>
 </sst>
 </file>
@@ -523,16 +541,16 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="topLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="18.14" customWidth="1"/>
     <col min="5" max="5" width="61.2" customWidth="1"/>
-    <col min="12" max="12" width="19.97" customWidth="1"/>
-    <col min="13" max="13" width="22.59" customWidth="1"/>
-    <col min="15" max="15" width="18.42" customWidth="1"/>
+    <col min="13" max="13" width="19.97" customWidth="1"/>
+    <col min="14" max="14" width="22.59" customWidth="1"/>
+    <col min="16" max="16" width="18.42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -560,31 +578,34 @@
       <c r="H1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>50</v>
       </c>
     </row>
@@ -604,13 +625,13 @@
       <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>200</v>
       </c>
     </row>
@@ -630,16 +651,16 @@
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>200</v>
       </c>
     </row>
@@ -662,22 +683,22 @@
       <c r="H4" s="0">
         <v>200</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>52</v>
       </c>
     </row>
@@ -694,8 +715,39 @@
       <c r="D5" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="I5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="N5" s="0" t="s">
         <v>63</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row ht="11.45" customHeight="1" r="6">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="N6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>